<commit_message>
update for general db
</commit_message>
<xml_diff>
--- a/docs/nsnqt_naming_vocabulary.xlsx
+++ b/docs/nsnqt_naming_vocabulary.xlsx
@@ -7,11 +7,12 @@
     <workbookView xWindow="360" yWindow="75" windowWidth="25815" windowHeight="16320"/>
   </bookViews>
   <sheets>
-    <sheet name="数据库字段中英文名称对照" sheetId="2" r:id="rId1"/>
-    <sheet name="常用英文术语定义" sheetId="3" r:id="rId2"/>
+    <sheet name="WSET" sheetId="4" r:id="rId1"/>
+    <sheet name="数据库字段中英文名称对照" sheetId="2" r:id="rId2"/>
+    <sheet name="常用英文术语定义" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="in_1" localSheetId="1">常用英文术语定义!$A$1:$B$51</definedName>
+    <definedName name="in_1" localSheetId="2">常用英文术语定义!$A$1:$B$51</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="279">
   <si>
     <t>[综合用词]</t>
   </si>
@@ -799,6 +800,265 @@
   </si>
   <si>
     <t>结算价（不前推）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据集</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基本资料</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上市股票一览</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wind代码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最新收盘价</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>总市值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>流通市值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>交易状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最新收盘价日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上市日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>证券类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上市板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上市交易所</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wind_code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sec_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>close_price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>total_market_value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mkt_cap_float</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>trade_status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ipo_date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>province</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sec_type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>listing_board</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exchange</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>参数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字段名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上市公司基本资料</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否保存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>省份</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>公司名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>成立日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>公司上市日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>已发行股票</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>股票类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注册资本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>法人代表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>信息披露人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注册地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>办公地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>邮政编码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电话</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>传真</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主页</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>英文名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>company_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>inception_date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>outstanding_shares</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>regcapital</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chairman</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>discloser</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>address</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>office</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zipcode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>telephone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fax</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>website</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>comp_name_eng</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>listedsecuritygeneralview</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>w.wset("listedsecuritygeneralview","sectorid=a001010100000000")</t>
+  </si>
+  <si>
+    <t>查询代码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>w.wset("listedcompanygenerayview","sectorid=a001010100000000")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>listedcompanygenerayview</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>index</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -823,12 +1083,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -845,8 +1111,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1147,9 +1419,435 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.75" customWidth="1"/>
+    <col min="6" max="6" width="70.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="27">
+      <c r="C3" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="B5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D5" t="s">
+        <v>273</v>
+      </c>
+      <c r="F5" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>278</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E6" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>218</v>
+      </c>
+      <c r="D7" t="s">
+        <v>229</v>
+      </c>
+      <c r="E7" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>219</v>
+      </c>
+      <c r="D8" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>220</v>
+      </c>
+      <c r="D9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>221</v>
+      </c>
+      <c r="D10" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D11" t="s">
+        <v>233</v>
+      </c>
+      <c r="E11" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>223</v>
+      </c>
+      <c r="D12" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>224</v>
+      </c>
+      <c r="D13" t="s">
+        <v>234</v>
+      </c>
+      <c r="E13" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>244</v>
+      </c>
+      <c r="D14" t="s">
+        <v>235</v>
+      </c>
+      <c r="E14" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="B15">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>225</v>
+      </c>
+      <c r="D15" t="s">
+        <v>236</v>
+      </c>
+      <c r="E15" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>226</v>
+      </c>
+      <c r="D16" t="s">
+        <v>237</v>
+      </c>
+      <c r="E16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>227</v>
+      </c>
+      <c r="D17" t="s">
+        <v>238</v>
+      </c>
+      <c r="E17" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" t="s">
+        <v>241</v>
+      </c>
+      <c r="D18" t="s">
+        <v>277</v>
+      </c>
+      <c r="F18" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="2">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="E19" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>246</v>
+      </c>
+      <c r="D20" t="s">
+        <v>261</v>
+      </c>
+      <c r="E20" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>247</v>
+      </c>
+      <c r="D21" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>248</v>
+      </c>
+      <c r="D22" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>249</v>
+      </c>
+      <c r="D23" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>250</v>
+      </c>
+      <c r="D24" t="s">
+        <v>263</v>
+      </c>
+      <c r="E24" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="B25">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>251</v>
+      </c>
+      <c r="D25" t="s">
+        <v>264</v>
+      </c>
+      <c r="E25" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="B26">
+        <v>7</v>
+      </c>
+      <c r="C26" t="s">
+        <v>252</v>
+      </c>
+      <c r="D26" t="s">
+        <v>265</v>
+      </c>
+      <c r="E26" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6">
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27" t="s">
+        <v>253</v>
+      </c>
+      <c r="D27" t="s">
+        <v>266</v>
+      </c>
+      <c r="E27" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6">
+      <c r="B28">
+        <v>9</v>
+      </c>
+      <c r="C28" t="s">
+        <v>254</v>
+      </c>
+      <c r="D28" t="s">
+        <v>267</v>
+      </c>
+      <c r="E28" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6">
+      <c r="B29">
+        <v>10</v>
+      </c>
+      <c r="C29" t="s">
+        <v>255</v>
+      </c>
+      <c r="D29" t="s">
+        <v>268</v>
+      </c>
+      <c r="E29" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6">
+      <c r="B30">
+        <v>11</v>
+      </c>
+      <c r="C30" t="s">
+        <v>256</v>
+      </c>
+      <c r="D30" t="s">
+        <v>269</v>
+      </c>
+      <c r="E30" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6">
+      <c r="B31">
+        <v>12</v>
+      </c>
+      <c r="C31" t="s">
+        <v>257</v>
+      </c>
+      <c r="D31" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6">
+      <c r="B32">
+        <v>13</v>
+      </c>
+      <c r="C32" t="s">
+        <v>258</v>
+      </c>
+      <c r="D32" t="s">
+        <v>271</v>
+      </c>
+      <c r="E32" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="B33">
+        <v>14</v>
+      </c>
+      <c r="C33" t="s">
+        <v>259</v>
+      </c>
+      <c r="D33" t="s">
+        <v>272</v>
+      </c>
+      <c r="E33" t="s">
+        <v>243</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
@@ -1661,7 +2359,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B51"/>
   <sheetViews>

</xml_diff>